<commit_message>
added event data to pipeline
</commit_message>
<xml_diff>
--- a/data_tables_concept.xlsx
+++ b/data_tables_concept.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\VSCProjects\EAI_SS24\EAI-SS24-finalProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6670A27C-AA78-46AE-AA82-60082A6BF876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D80A6D-C4B9-41A8-BCA3-60712AF54DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{0FF859AC-B36A-4DF3-AA38-436474F7287D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>DATA.db</t>
   </si>
@@ -134,9 +134,6 @@
     <t>bool</t>
   </si>
   <si>
-    <t>int?</t>
-  </si>
-  <si>
     <t>month</t>
   </si>
   <si>
@@ -149,12 +146,6 @@
     <t>onehotencoding</t>
   </si>
   <si>
-    <t>feiertag</t>
-  </si>
-  <si>
-    <t>wochenmarkt</t>
-  </si>
-  <si>
     <t>feiertage und mehr</t>
   </si>
   <si>
@@ -165,13 +156,47 @@
   </si>
   <si>
     <t>table 5</t>
+  </si>
+  <si>
+    <t>workday</t>
+  </si>
+  <si>
+    <t>hollyday</t>
+  </si>
+  <si>
+    <r>
+      <t>timestamp/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>date</t>
+    </r>
+  </si>
+  <si>
+    <t>geen_market</t>
+  </si>
+  <si>
+    <t>special_market</t>
+  </si>
+  <si>
+    <t>LEED FEATUERS FÜR DIESE ERSTELLEN???</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -210,8 +235,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,6 +285,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -370,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,15 +470,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -444,12 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,7 +497,13 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -803,65 +841,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551F3403-8894-4B5D-AF9E-113FD965DF4A}">
-  <dimension ref="A1:N31"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="24.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="14.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="14.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="12" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="27" t="s">
-        <v>41</v>
+      <c r="C3" s="23" t="s">
+        <v>38</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="H3" s="14"/>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
       <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="12"/>
-    </row>
-    <row r="4" spans="1:14" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L3" s="12"/>
+    </row>
+    <row r="4" spans="1:12" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="24" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="30" t="s">
+      <c r="E4" s="26" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="3" t="s">
@@ -870,7 +905,7 @@
       <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="16" t="s">
         <v>16</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -882,30 +917,24 @@
       <c r="K4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="25" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="27" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="6" t="s">
@@ -914,7 +943,7 @@
       <c r="G5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -926,244 +955,253 @@
       <c r="K5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="M5" s="5" t="s">
+      <c r="L5" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="B10" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="12"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D8" s="24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="26"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="10" t="s">
+      <c r="C16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="5"/>
+      <c r="B28" s="7"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="12"/>
-      <c r="H11" s="32"/>
-      <c r="I11" s="32"/>
-      <c r="J11" s="32"/>
-      <c r="K11" s="32"/>
-      <c r="L11" s="32"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="B30" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="12"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="12"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A17" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="B31" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="12"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="18" t="s">
+      <c r="B32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A9:D9"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>